<commit_message>
umls, demo, test cases and source code added, bugs fixed
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tarun\eclipse-workspace\TheGameOfLife\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D69BACBC-66CB-40CA-8C7C-95C2AE63FB2B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE102610-39CD-44F6-9023-6D934A074271}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{9D2504BA-DD35-49A0-9980-0DB3BABEC231}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="54">
   <si>
     <t>Board</t>
   </si>
@@ -102,29 +102,6 @@
     <t>Refactoring</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>NOTE:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Pair programming is employed most of the time</t>
-    </r>
-  </si>
-  <si>
     <t>Test Cases updated</t>
   </si>
   <si>
@@ -165,13 +142,58 @@
   </si>
   <si>
     <t>Game superclass to control gameplay</t>
+  </si>
+  <si>
+    <t>Game changes</t>
+  </si>
+  <si>
+    <t>Inputs</t>
+  </si>
+  <si>
+    <t>Loops for movement</t>
+  </si>
+  <si>
+    <t>Failsafe/Exception handling</t>
+  </si>
+  <si>
+    <t>Decks to use logic from tree/node</t>
+  </si>
+  <si>
+    <t>Merge functionality</t>
+  </si>
+  <si>
+    <t>Test Cases and UML update</t>
+  </si>
+  <si>
+    <t>Block Logic updated</t>
+  </si>
+  <si>
+    <t>Refactoring for more polymorphism</t>
+  </si>
+  <si>
+    <t>Block differences</t>
+  </si>
+  <si>
+    <t>Final checks</t>
+  </si>
+  <si>
+    <t>Cleaning/refactoring</t>
+  </si>
+  <si>
+    <t>Clean code</t>
+  </si>
+  <si>
+    <t>Readible code</t>
+  </si>
+  <si>
+    <t>Submission</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,16 +238,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,6 +264,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -278,26 +298,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3"/>
-    <xf numFmtId="16" fontId="1" fillId="5" borderId="0" xfId="4" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
+    <cellStyle name="20% - Accent1" xfId="5" builtinId="30"/>
     <cellStyle name="40% - Accent5" xfId="4" builtinId="47"/>
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -614,7 +635,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D601F7A5-B89E-4D14-8E7A-528DF2943E0F}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
@@ -640,7 +661,7 @@
         <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>19</v>
@@ -648,43 +669,43 @@
       <c r="F1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
-        <v>27</v>
+      <c r="A2" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="9">
+      <c r="A3" s="7">
         <v>43388</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="B4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="3" t="s">
@@ -692,13 +713,13 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="9">
+      <c r="A5" s="7">
         <v>43395</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -707,28 +728,28 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="9">
+      <c r="A7" s="7">
         <v>43402</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="8" t="s">
+      <c r="B7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>18</v>
@@ -736,24 +757,24 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
+      <c r="A9" s="7">
         <v>43409</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -761,79 +782,130 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="7" t="s">
+      <c r="B10" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="C10" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+      <c r="A11" s="7">
         <v>43416</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C12" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+      <c r="A13" s="7">
         <v>43423</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="8" t="s">
+      <c r="B13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
+      <c r="B14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
+      <c r="A15" s="7">
         <v>43430</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
+      <c r="B16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="7">
         <v>43437</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
+      <c r="B18" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="7">
         <v>43444</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>43451</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>25</v>
+      <c r="B21" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>